<commit_message>
Entered initial sprint 1 data
</commit_message>
<xml_diff>
--- a/Sprint-Backlog.xlsx
+++ b/Sprint-Backlog.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07FD5D8-548D-4E24-AC99-D9D38F2DAC70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +19,116 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>As a member of a shared living space, I want to keep track of communal living expenses in order to stop relying on the “I owe you” system between everybody.</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>As a member of a shared living space, I want to be able to estimate how much will owe for my portion of the monthly bills so that I can properly set aside/save funds in advance.</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>As someone with many different types of expenses, I want to be able to manually track other types of expenses and bills and which roommates are responsible for them, so that I manage all my expenses.</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to set the amount each person owes for each bill by splitting evenly, setting specific dollar amounts, or assigning percentages so that I can fairly assign payments between roommates.</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>As a user with many different expenses, I want to be able to see how much I owe over certain time periods (monthly, weekly, etc.) and who is charging me for what so that I can be sure I am being charged correctly.</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>As a user, if I don’t have the cash to pay bills on time I’d like to be able to pay either in order of a) the age of the debt, or b) my own set priorities. These would allow convenience to me, and fairness to my creditors.</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to input payments I make in person (via cash or check) so that I have flexibility in my payment options.</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>As user I want to be able to dispute charges and message who ever assessed them if they aren’t correct so that I don’t get charged incorrectly and can resolve the problem anywhere.</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>As a member of a shared living space, I want to have a communal shopping list to track what need to be purchased and who gets charged for the purchases so the time without certain items is reduced and everyone charged fairly.</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>As a member of a shared living space, I want a communal “bulletin board” board to post messages for the room (e.g. take out the trash, clean dishes etc) to communicate with all roommates more easily.</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>As someone with several shared spaces I want to be able to create my own “room” so I can add and remove members as needed.</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to access the site from anywhere without any geographic requirements or too much validation of location so that my privacy is protected.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Subtype</t>
+  </si>
+  <si>
+    <t>Story points</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Contribution</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +136,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +178,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +472,197 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="38.19921875" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" customWidth="1"/>
+    <col min="5" max="5" width="12.1328125" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12.265625" customWidth="1"/>
+    <col min="8" max="8" width="13.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Invalid entry" promptTitle="Priority" prompt="Choose an option from the dropdown." sqref="E2:E13" xr:uid="{D166CE97-B1D1-4DE9-8A72-37077492B471}">
+      <formula1>"High, Medium, Low"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{AB09CA09-718F-45E4-935D-F636D6BED0FB}">
+      <formula1>"Functional, Non-functional"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{3679F50C-42D2-401E-8554-D75F273E62AA}">
+      <formula1>"Bug, Technical work, Knowledge acquisition"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" errorTitle="Error" error="Invalid input" promptTitle="Status" prompt="Choose an option from the dropdown." sqref="F2:F1048576" xr:uid="{90BACBB7-86D6-4076-A890-CF66BAD408FD}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{556C45FD-623C-4BB3-9007-E7763D8161BF}">
+      <formula1>"Aiden, Josh, Matt P, Matt A, Durgin"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Filled out sprint backlog sheet
</commit_message>
<xml_diff>
--- a/Sprint-Backlog.xlsx
+++ b/Sprint-Backlog.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07FD5D8-548D-4E24-AC99-D9D38F2DAC70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F110FF4-BB33-44B8-B4D8-F27A9012B533}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>001</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Contribution</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Technical work</t>
   </si>
 </sst>
 </file>
@@ -476,17 +482,20 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="9.06640625" customWidth="1"/>
     <col min="2" max="2" width="38.19921875" customWidth="1"/>
+    <col min="3" max="3" width="15.73046875" customWidth="1"/>
     <col min="4" max="4" width="19.86328125" customWidth="1"/>
     <col min="5" max="5" width="12.1328125" customWidth="1"/>
     <col min="6" max="6" width="16.59765625" customWidth="1"/>
     <col min="7" max="7" width="12.265625" customWidth="1"/>
     <col min="8" max="8" width="13.86328125" customWidth="1"/>
+    <col min="9" max="16384" width="9.06640625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -522,8 +531,17 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
       <c r="E2" t="s">
         <v>2</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.45">
@@ -533,8 +551,17 @@
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
       <c r="E3" t="s">
         <v>5</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
@@ -544,8 +571,17 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
       <c r="E4" t="s">
         <v>2</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
@@ -555,8 +591,17 @@
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
       <c r="E5" t="s">
         <v>2</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
@@ -566,8 +611,17 @@
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
       <c r="E6" t="s">
         <v>5</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
@@ -577,8 +631,17 @@
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
       <c r="E7" t="s">
         <v>5</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
@@ -588,8 +651,17 @@
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" t="s">
         <v>2</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
@@ -599,8 +671,17 @@
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
       <c r="E9" t="s">
         <v>5</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
@@ -610,8 +691,17 @@
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
       <c r="E10" t="s">
         <v>2</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
@@ -621,8 +711,17 @@
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
       <c r="E11" t="s">
         <v>5</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
@@ -632,8 +731,17 @@
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
       <c r="E12" t="s">
         <v>2</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="57" x14ac:dyDescent="0.45">
@@ -643,8 +751,17 @@
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
       <c r="E13" t="s">
         <v>5</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -664,5 +781,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>